<commit_message>
Connexion front/back et implémentation des fonctions du front
</commit_message>
<xml_diff>
--- a/BackEnd/bdd/Dataset_movies.xlsx
+++ b/BackEnd/bdd/Dataset_movies.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28412"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://devinci-my.sharepoint.com/personal/romain_paupe_edu_devinci_fr/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nurno\FinalProject\BackEnd\bdd\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="14_{5B4C9CF2-3F68-4676-B0C7-5919F8B15E99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B80B3A7D-9AE2-4610-B28B-2BB4BB810C3E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F2EFA5F-956D-492E-85C2-28E066F44E2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{6FAA606D-731C-4CD4-912D-A6E3961135DE}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{6FAA606D-731C-4CD4-912D-A6E3961135DE}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="72">
   <si>
     <t>ID</t>
   </si>
@@ -266,6 +266,30 @@
   </si>
   <si>
     <t>Andy Dufresne, a banker falsely imprisoned for his wife's murder, befriends fellow inmate Ellis Redding while serving a life sentence in Shawshank State Penitentiary. Over time, Andy's intelligence and resourcefulness help transform the prison, offering hope and redemption to its inhabitants.</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/en/a/ab/La_La_Land_%28film%29.png</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/en/2/2e/Inception_%282010%29_theatrical_poster.jpg</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/en/1/1c/The_Dark_Knight_%282008_film%29.jpg</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/en/b/bc/Interstellar_film_poster.jpg</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/en/5/53/Parasite_%282019_film%29.png</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/en/a/a6/Once_Upon_a_Time_in_Hollywood_poster.png</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/vi/a/a6/The_Grand_Budapest_Hotel_Poster.jpg?20150116031701</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/en/8/81/ShawshankRedemptionMoviePoster.jpg</t>
   </si>
 </sst>
 </file>
@@ -798,21 +822,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48F004E0-B490-4E76-89E7-EE54B00126DB}">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="72" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="98" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="2" max="2" width="44" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" customWidth="1"/>
-    <col min="4" max="4" width="19.42578125" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="26.42578125" customWidth="1"/>
-    <col min="7" max="8" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="12.88671875" customWidth="1"/>
+    <col min="4" max="4" width="19.44140625" customWidth="1"/>
+    <col min="5" max="5" width="14.109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="26.44140625" customWidth="1"/>
+    <col min="7" max="8" width="16.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.95">
+    <row r="1" spans="1:8" ht="15.6">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -838,7 +862,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="14.45">
+    <row r="2" spans="1:8" ht="14.4">
       <c r="A2">
         <v>0</v>
       </c>
@@ -864,7 +888,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="14.45">
+    <row r="3" spans="1:8" ht="14.4">
       <c r="A3">
         <v>1</v>
       </c>
@@ -890,7 +914,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="14.45">
+    <row r="4" spans="1:8" ht="14.4">
       <c r="A4">
         <v>2</v>
       </c>
@@ -938,6 +962,9 @@
       <c r="G5" t="s">
         <v>30</v>
       </c>
+      <c r="H5" s="4" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="6" spans="1:8" ht="15" customHeight="1">
       <c r="A6">
@@ -961,6 +988,9 @@
       <c r="G6" t="s">
         <v>34</v>
       </c>
+      <c r="H6" s="4" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="7" spans="1:8" ht="15" customHeight="1">
       <c r="A7">
@@ -984,6 +1014,9 @@
       <c r="G7" t="s">
         <v>39</v>
       </c>
+      <c r="H7" s="4" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="8" spans="1:8" ht="15" customHeight="1">
       <c r="A8">
@@ -1007,6 +1040,9 @@
       <c r="G8" t="s">
         <v>43</v>
       </c>
+      <c r="H8" s="4" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="9" spans="1:8" ht="15" customHeight="1">
       <c r="A9">
@@ -1030,6 +1066,9 @@
       <c r="G9" t="s">
         <v>48</v>
       </c>
+      <c r="H9" s="4" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="10" spans="1:8" ht="15" customHeight="1">
       <c r="A10">
@@ -1053,6 +1092,9 @@
       <c r="G10" t="s">
         <v>53</v>
       </c>
+      <c r="H10" s="4" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="11" spans="1:8" ht="15" customHeight="1">
       <c r="A11">
@@ -1076,6 +1118,9 @@
       <c r="G11" t="s">
         <v>58</v>
       </c>
+      <c r="H11" s="4" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="12" spans="1:8" ht="15" customHeight="1">
       <c r="A12">
@@ -1098,6 +1143,9 @@
       </c>
       <c r="G12" t="s">
         <v>63</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1107,30 +1155,21 @@
     <hyperlink ref="F3" r:id="rId3" tooltip="Daniel Radcliffe" display="https://en.wikipedia.org/wiki/Daniel_Radcliffe" xr:uid="{1EFDD90E-2CED-468C-A869-5EE029DFD180}"/>
     <hyperlink ref="H3" r:id="rId4" xr:uid="{B343B661-A4B8-473D-B17C-4633B333D124}"/>
     <hyperlink ref="D4" r:id="rId5" tooltip="Martin Scorsese" display="https://en.wikipedia.org/wiki/Martin_Scorsese" xr:uid="{1491D2EB-205B-458B-B130-D28EF5DE2537}"/>
+    <hyperlink ref="H7" r:id="rId6" xr:uid="{C1E3C811-CBA6-4769-A6A5-3C533643ACF2}"/>
+    <hyperlink ref="H5" r:id="rId7" xr:uid="{5E2FC834-E23B-4B01-8C15-E6EDBC6C5D3A}"/>
+    <hyperlink ref="H6" r:id="rId8" xr:uid="{5B50B129-B63E-4ED9-94FC-F2BAB569C3C9}"/>
+    <hyperlink ref="H8" r:id="rId9" xr:uid="{E7F326F4-AFA1-4403-B8BB-C5F0AF4FCD08}"/>
+    <hyperlink ref="H9" r:id="rId10" xr:uid="{A0050659-D517-42DA-9D65-51C1A88450E0}"/>
+    <hyperlink ref="H10" r:id="rId11" xr:uid="{F17A520F-CE16-4AC0-BB1D-5FA3A1C233F2}"/>
+    <hyperlink ref="H11" r:id="rId12" xr:uid="{F9CB8D8D-05B8-4D6D-9CCC-25CDA40CD29D}"/>
+    <hyperlink ref="H12" r:id="rId13" xr:uid="{A7256D86-D53F-4613-964C-35714713CE4F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId6"/>
+  <drawing r:id="rId14"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="c62e4d98-e61d-45dd-b89d-68f8f7a6103d" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F600ED0C1E48C74DB12CA09925A832A9" ma:contentTypeVersion="18" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="d5aa9ee7efaaebb626b7bd83d6c79e53">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="c62e4d98-e61d-45dd-b89d-68f8f7a6103d" xmlns:ns4="cf0ce9cc-f47c-412f-a632-ecb5e972046b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="918565ae1b5366c1335c6d5213bac21b" ns3:_="" ns4:_="">
     <xsd:import namespace="c62e4d98-e61d-45dd-b89d-68f8f7a6103d"/>
@@ -1383,14 +1422,56 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="c62e4d98-e61d-45dd-b89d-68f8f7a6103d" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{45E091B0-B870-4ADC-AC58-266179D08CB0}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2671738-1B77-4231-941C-27D2852FBB14}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="c62e4d98-e61d-45dd-b89d-68f8f7a6103d"/>
+    <ds:schemaRef ds:uri="cf0ce9cc-f47c-412f-a632-ecb5e972046b"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3170A0F9-4E43-45C2-A19A-5A74EFD6433F}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3170A0F9-4E43-45C2-A19A-5A74EFD6433F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2671738-1B77-4231-941C-27D2852FBB14}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{45E091B0-B870-4ADC-AC58-266179D08CB0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="c62e4d98-e61d-45dd-b89d-68f8f7a6103d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>